<commit_message>
[TABELAS E HISTOGRAMAS] TODOS PRONTOS
</commit_message>
<xml_diff>
--- a/Cenario1/FrequenciaTECOUT.xlsx
+++ b/Cenario1/FrequenciaTECOUT.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="FrequenciaTECOUT" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -638,11 +638,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>FrequenciaTECOUT!$B$1</c:f>
+              <c:f>FrequenciaTECOUT!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> Frequencia </c:v>
+                  <c:v> Frequencia Relativa </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -673,24 +673,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FrequenciaTECOUT!$B$2:$B$6</c:f>
+              <c:f>FrequenciaTECOUT!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>136</c:v>
+                  <c:v>0.18784529999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>135</c:v>
+                  <c:v>0.18646409</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>146</c:v>
+                  <c:v>0.20165746000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>159</c:v>
+                  <c:v>0.21961325000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>137</c:v>
+                  <c:v>0.18922652000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -705,11 +705,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="129091072"/>
-        <c:axId val="129092608"/>
+        <c:axId val="188949632"/>
+        <c:axId val="188951168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="129091072"/>
+        <c:axId val="188949632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -718,7 +718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129092608"/>
+        <c:crossAx val="188951168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -726,7 +726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129092608"/>
+        <c:axId val="188951168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +737,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129091072"/>
+        <c:crossAx val="188949632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>